<commit_message>
Update CSS and AcceptanceCriteria.xlsx
</commit_message>
<xml_diff>
--- a/AcceptanceCriteria.xlsx
+++ b/AcceptanceCriteria.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polytechintl-my.sharepoint.com/personal/o_mahmoud22026_pi_tn/Documents/_IRM-2-2-S1/C# .NET/Projet/CloudXForum/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{5FF49E68-E68C-426F-A2C2-D9A44D4D6CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CBF0F0EB-46E4-42B5-B7C2-45913D96B541}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="8_{5FF49E68-E68C-426F-A2C2-D9A44D4D6CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{56835B21-0FB3-4415-8924-DED09AD90DC3}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{CFCB619F-005A-42C7-9291-1F4ED48D634C}"/>
   </bookViews>
@@ -894,7 +894,7 @@
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1078,7 +1078,7 @@
         <v>26</v>
       </c>
       <c r="C19" s="7">
-        <v>0</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -1086,7 +1086,7 @@
         <v>27</v>
       </c>
       <c r="C20" s="7">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -1094,7 +1094,7 @@
         <v>28</v>
       </c>
       <c r="C21" s="7">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -1151,7 +1151,7 @@
         <v>37</v>
       </c>
       <c r="C27" s="7">
-        <v>100</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -1159,7 +1159,7 @@
         <v>38</v>
       </c>
       <c r="C28" s="7">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -1208,8 +1208,8 @@
     <cfRule type="iconSet" priority="1">
       <iconSet iconSet="3Symbols" showValue="0">
         <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="0" gte="0"/>
-        <cfvo type="percent" val="100"/>
+        <cfvo type="num" val="0" gte="0"/>
+        <cfvo type="num" val="100"/>
       </iconSet>
     </cfRule>
   </conditionalFormatting>

</xml_diff>